<commit_message>
allow the runControl file to run multiple plans
</commit_message>
<xml_diff>
--- a/RunControl_initRuns.xlsx
+++ b/RunControl_initRuns.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -1273,10 +1273,10 @@
   <dimension ref="A1:AN15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="P6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2703,8 +2703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2827,8 +2827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2869,7 +2869,7 @@
         <v>105</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="C3">
         <v>8</v>

</xml_diff>

<commit_message>
add control over whether negative contribution is allowed
</commit_message>
<xml_diff>
--- a/RunControl_initRuns.xlsx
+++ b/RunControl_initRuns.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\PenSim-Projects\Model_Main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Model_Main\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="185">
   <si>
     <t>Sheet #</t>
   </si>
@@ -199,9 +199,6 @@
     <t>Method 1 (PSERS): The difference between expected and actual investment return will be realized over s.year years. (realize 1/s.year each year)</t>
   </si>
   <si>
-    <t>Method 2 (TPAF):  "MA" for preset value; "AL" for being equal to initial liability</t>
-  </si>
-  <si>
     <t>Method 2 (TPAF): expected market value at 0. Set to the same value as MA_0 by default. expected market value at 0. Set to the same value as MA_0 by default</t>
   </si>
   <si>
@@ -572,6 +569,21 @@
   </si>
   <si>
     <t>Fixed Return Fixed discount rate and investment return, 7.5% each; Typical</t>
+  </si>
+  <si>
+    <t>Non-Negative ADC and ERC</t>
+  </si>
+  <si>
+    <t>nonNegC</t>
+  </si>
+  <si>
+    <t>How initial MA is determined</t>
+  </si>
+  <si>
+    <t>"MA" for preset value; "AL" for being equal to initial liability;""AL_pct being % of AL</t>
+  </si>
+  <si>
+    <t>MA_0_pct</t>
   </si>
 </sst>
 </file>
@@ -705,7 +717,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -745,10 +757,16 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -757,17 +775,14 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1129,14 +1144,14 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875"/>
-    <col min="2" max="2" width="16.6640625"/>
-    <col min="3" max="1025" width="8.5546875"/>
+    <col min="1" max="1" width="7.5703125"/>
+    <col min="2" max="2" width="16.7109375"/>
+    <col min="3" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1144,7 +1159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1152,7 +1167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1160,7 +1175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1187,77 +1202,77 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.5546875"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1270,37 +1285,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN15"/>
+  <dimension ref="A1:AP15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="AE6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="AJ15" sqref="AJ15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.44140625"/>
-    <col min="2" max="2" width="98.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="24.44140625"/>
-    <col min="10" max="11" width="17.44140625"/>
-    <col min="12" max="12" width="16.109375"/>
-    <col min="13" max="14" width="21.44140625"/>
-    <col min="15" max="15" width="24.5546875"/>
+    <col min="1" max="1" width="54.42578125"/>
+    <col min="2" max="2" width="98.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="24.42578125"/>
+    <col min="10" max="11" width="17.42578125"/>
+    <col min="12" max="12" width="16.140625"/>
+    <col min="13" max="14" width="21.42578125"/>
+    <col min="15" max="15" width="24.5703125"/>
     <col min="16" max="16" width="16"/>
-    <col min="17" max="21" width="12.6640625"/>
-    <col min="22" max="22" width="11.109375" customWidth="1"/>
-    <col min="23" max="32" width="12.6640625"/>
-    <col min="34" max="34" width="12.6640625"/>
-    <col min="35" max="37" width="27.109375"/>
-    <col min="38" max="38" width="20.6640625"/>
-    <col min="39" max="39" width="26.88671875"/>
-    <col min="40" max="40" width="16"/>
-    <col min="41" max="1027" width="8.5546875"/>
+    <col min="17" max="21" width="12.7109375"/>
+    <col min="22" max="22" width="11.140625" customWidth="1"/>
+    <col min="23" max="32" width="12.7109375"/>
+    <col min="37" max="37" width="12.7109375"/>
+    <col min="38" max="39" width="27.140625"/>
+    <col min="40" max="40" width="26.85546875"/>
+    <col min="42" max="42" width="16"/>
+    <col min="43" max="1029" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1308,8 +1322,9 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
-    </row>
-    <row r="2" spans="1:40" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="AH1" s="1"/>
+    </row>
+    <row r="2" spans="1:42" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -1371,17 +1386,23 @@
         <v>40</v>
       </c>
       <c r="AH2" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AI2" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AI2" s="6"/>
-      <c r="AJ2" s="6"/>
-      <c r="AK2" s="6"/>
       <c r="AL2" s="6"/>
-      <c r="AN2" s="4" t="s">
+      <c r="AM2" s="6"/>
+      <c r="AO2" s="6"/>
+      <c r="AP2" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:40" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:42" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -1416,239 +1437,248 @@
         <v>53</v>
       </c>
       <c r="AI3" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="AJ3" s="4"/>
+      <c r="AM3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AK3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AM3" s="4" t="s">
+      <c r="AP3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AN3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:42" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:40" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="29" t="s">
+      <c r="E4" s="25"/>
+      <c r="F4" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30" t="s">
+      <c r="G4" s="26"/>
+      <c r="H4" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="25" t="s">
+      <c r="I4" s="27"/>
+      <c r="J4" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="25"/>
-      <c r="J4" s="26" t="s">
+      <c r="K4" s="28"/>
+      <c r="L4" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="K4" s="26"/>
-      <c r="L4" s="25" t="s">
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="26" t="s">
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="T4" s="26"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="23" t="s">
+      <c r="W4" s="29"/>
+      <c r="X4" s="29"/>
+      <c r="Y4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="W4" s="23"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="7" t="s">
+      <c r="Z4" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="Z4" s="27" t="s">
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="28" t="s">
+      <c r="AD4" s="30"/>
+      <c r="AE4" s="30"/>
+      <c r="AF4" s="30"/>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="23"/>
+      <c r="AI4" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="AD4" s="28"/>
-      <c r="AE4" s="28"/>
-      <c r="AF4" s="28"/>
-      <c r="AG4" s="17"/>
-      <c r="AH4" s="23" t="s">
+      <c r="AJ4" s="29"/>
+      <c r="AK4" s="29"/>
+      <c r="AL4" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="AI4" s="23"/>
-      <c r="AJ4" s="24" t="s">
+      <c r="AM4" s="31"/>
+      <c r="AN4" s="31"/>
+      <c r="AO4" s="31"/>
+      <c r="AP4" s="31"/>
+    </row>
+    <row r="5" spans="1:42" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="AK4" s="24"/>
-      <c r="AL4" s="24"/>
-      <c r="AM4" s="24"/>
-      <c r="AN4" s="24"/>
-    </row>
-    <row r="5" spans="1:40" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="B5" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="C5" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="K5" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="L5" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="M5" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="N5" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="O5" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="P5" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="Q5" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="R5" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="S5" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="S5" s="9" t="s">
+      <c r="T5" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="T5" s="9" t="s">
+      <c r="U5" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="U5" s="9" t="s">
+      <c r="V5" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="W5" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="V5" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="W5" s="9" t="s">
+      <c r="X5" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="X5" s="9" t="s">
+      <c r="Y5" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="Y5" s="9" t="s">
+      <c r="Z5" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="Z5" s="9" t="s">
+      <c r="AA5" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="AA5" s="9" t="s">
+      <c r="AB5" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="AB5" s="9" t="s">
+      <c r="AC5" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="AC5" s="9" t="s">
+      <c r="AD5" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="AD5" s="9" t="s">
+      <c r="AE5" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="AE5" s="9" t="s">
+      <c r="AF5" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="AF5" s="9" t="s">
+      <c r="AG5" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="AH5" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AI5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AJ5" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="AK5" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG5" s="9" t="s">
+      <c r="AL5" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM5" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN5" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="AO5" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP5" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>162</v>
       </c>
-      <c r="AH5" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="AI5" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="AJ5" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="AK5" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AL5" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="AM5" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="AN5" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>163</v>
-      </c>
       <c r="B6" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C6" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" t="s">
         <v>110</v>
       </c>
-      <c r="E6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>111</v>
-      </c>
-      <c r="I6" t="s">
-        <v>112</v>
       </c>
       <c r="J6" s="12">
         <v>0</v>
@@ -1687,7 +1717,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V6" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="W6" s="12">
         <v>7.4999999999999997E-2</v>
@@ -1696,19 +1726,19 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Z6" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA6" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="AA6" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="AB6">
         <v>30</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AD6" s="14">
         <v>0.25</v>
@@ -1722,56 +1752,62 @@
       <c r="AG6" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="AH6">
+      <c r="AH6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ6" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK6">
         <v>200</v>
       </c>
-      <c r="AI6" s="2" t="s">
+      <c r="AL6" t="s">
         <v>117</v>
       </c>
-      <c r="AJ6" t="s">
-        <v>118</v>
-      </c>
-      <c r="AK6">
+      <c r="AM6">
         <v>10</v>
       </c>
-      <c r="AL6" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>200</v>
       </c>
-      <c r="AN6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C7" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" t="s">
         <v>110</v>
       </c>
-      <c r="E7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F7" t="s">
-        <v>110</v>
-      </c>
-      <c r="G7" t="s">
-        <v>110</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>111</v>
-      </c>
-      <c r="I7" t="s">
-        <v>112</v>
       </c>
       <c r="J7" s="12">
         <v>0</v>
@@ -1810,7 +1846,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="W7" s="12">
         <v>5.5E-2</v>
@@ -1819,19 +1855,19 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Z7" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA7" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="AB7">
         <v>30</v>
       </c>
       <c r="AC7" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AD7" s="14">
         <v>0.25</v>
@@ -1845,56 +1881,62 @@
       <c r="AG7" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="AH7">
+      <c r="AH7" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI7" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ7" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK7">
         <v>200</v>
       </c>
-      <c r="AI7" s="2" t="s">
+      <c r="AL7" t="s">
         <v>117</v>
       </c>
-      <c r="AJ7" t="s">
-        <v>118</v>
-      </c>
-      <c r="AK7">
+      <c r="AM7">
         <v>10</v>
       </c>
-      <c r="AL7" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM7">
+      <c r="AN7">
         <v>200</v>
       </c>
-      <c r="AN7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO7" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C8" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" t="s">
         <v>110</v>
       </c>
-      <c r="E8" t="s">
-        <v>110</v>
-      </c>
-      <c r="F8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G8" t="s">
-        <v>110</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>111</v>
-      </c>
-      <c r="I8" t="s">
-        <v>112</v>
       </c>
       <c r="J8" s="12">
         <v>0</v>
@@ -1933,7 +1975,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V8" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="W8" s="12">
         <v>9.5000000000000001E-2</v>
@@ -1942,19 +1984,19 @@
         <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Z8" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA8" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="AA8" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="AB8">
         <v>30</v>
       </c>
       <c r="AC8" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AD8" s="14">
         <v>0.25</v>
@@ -1968,56 +2010,62 @@
       <c r="AG8" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="AH8">
+      <c r="AH8" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI8" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ8" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK8">
         <v>200</v>
       </c>
-      <c r="AI8" s="2" t="s">
+      <c r="AL8" t="s">
         <v>117</v>
       </c>
-      <c r="AJ8" t="s">
-        <v>118</v>
-      </c>
-      <c r="AK8">
+      <c r="AM8">
         <v>10</v>
       </c>
-      <c r="AL8" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM8">
+      <c r="AN8">
         <v>200</v>
       </c>
-      <c r="AN8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO8" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C9" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" t="s">
         <v>110</v>
       </c>
-      <c r="E9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F9" t="s">
-        <v>110</v>
-      </c>
-      <c r="G9" t="s">
-        <v>110</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>111</v>
-      </c>
-      <c r="I9" t="s">
-        <v>112</v>
       </c>
       <c r="J9" s="12">
         <v>0</v>
@@ -2056,7 +2104,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V9" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="W9" s="12">
         <v>7.4999999999999997E-2</v>
@@ -2065,19 +2113,19 @@
         <v>0.12</v>
       </c>
       <c r="Y9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Z9" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA9" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="AA9" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="AB9">
         <v>30</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AD9" s="14">
         <v>0.25</v>
@@ -2091,56 +2139,62 @@
       <c r="AG9" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="AH9">
+      <c r="AH9" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI9" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ9" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK9">
         <v>200</v>
       </c>
-      <c r="AI9" s="2" t="s">
+      <c r="AL9" t="s">
         <v>117</v>
       </c>
-      <c r="AJ9" t="s">
-        <v>118</v>
-      </c>
-      <c r="AK9">
+      <c r="AM9">
         <v>10</v>
       </c>
-      <c r="AL9" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM9">
+      <c r="AN9">
         <v>200</v>
       </c>
-      <c r="AN9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C10" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" t="s">
         <v>110</v>
       </c>
-      <c r="E10" t="s">
-        <v>110</v>
-      </c>
-      <c r="F10" t="s">
-        <v>110</v>
-      </c>
-      <c r="G10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>111</v>
-      </c>
-      <c r="I10" t="s">
-        <v>112</v>
       </c>
       <c r="J10" s="12">
         <v>0</v>
@@ -2179,7 +2233,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V10" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="W10" s="12">
         <v>0</v>
@@ -2188,19 +2242,19 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Z10" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA10" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="AA10" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="AB10">
         <v>30</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AD10" s="14">
         <v>0.25</v>
@@ -2214,56 +2268,62 @@
       <c r="AG10" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="AH10">
+      <c r="AH10" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI10" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ10" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK10">
         <v>200</v>
       </c>
-      <c r="AI10" s="2" t="s">
+      <c r="AL10" t="s">
         <v>117</v>
       </c>
-      <c r="AJ10" t="s">
-        <v>118</v>
-      </c>
-      <c r="AK10">
+      <c r="AM10">
         <v>10</v>
       </c>
-      <c r="AL10" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM10">
+      <c r="AN10">
         <v>200</v>
       </c>
-      <c r="AN10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO10" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C11" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" t="s">
         <v>110</v>
       </c>
-      <c r="E11" t="s">
-        <v>110</v>
-      </c>
-      <c r="F11" t="s">
-        <v>110</v>
-      </c>
-      <c r="G11" t="s">
-        <v>110</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>111</v>
-      </c>
-      <c r="I11" t="s">
-        <v>112</v>
       </c>
       <c r="J11" s="12">
         <v>0</v>
@@ -2302,7 +2362,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V11" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="W11" s="12">
         <v>7.4999999999999997E-2</v>
@@ -2311,19 +2371,19 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Z11" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA11" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="AA11" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="AB11">
         <v>30</v>
       </c>
       <c r="AC11" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AD11" s="14">
         <v>0.25</v>
@@ -2337,59 +2397,71 @@
       <c r="AG11" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AH11">
+      <c r="AH11" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI11" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ11" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK11">
         <v>200</v>
       </c>
-      <c r="AI11" s="2" t="s">
+      <c r="AL11" t="s">
         <v>117</v>
       </c>
-      <c r="AJ11" t="s">
-        <v>118</v>
-      </c>
-      <c r="AK11">
+      <c r="AM11">
         <v>10</v>
       </c>
-      <c r="AL11" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM11">
+      <c r="AN11">
         <v>200</v>
       </c>
-      <c r="AN11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO11" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B12" s="22"/>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AH12" s="21"/>
+      <c r="AJ12" s="19"/>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AH13" s="21"/>
+      <c r="AJ13" s="19"/>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C14" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" t="s">
         <v>110</v>
       </c>
-      <c r="E14" t="s">
-        <v>110</v>
-      </c>
-      <c r="F14" t="s">
-        <v>110</v>
-      </c>
-      <c r="G14" t="s">
-        <v>110</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>111</v>
-      </c>
-      <c r="I14" t="s">
-        <v>112</v>
       </c>
       <c r="J14" s="12">
         <v>0</v>
@@ -2428,7 +2500,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V14" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="W14" s="12">
         <v>7.4999999999999997E-2</v>
@@ -2437,19 +2509,19 @@
         <v>0</v>
       </c>
       <c r="Y14" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z14" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="Z14" s="2" t="s">
+      <c r="AA14" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="AA14" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="AB14">
         <v>10</v>
       </c>
       <c r="AC14" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AD14" s="14">
         <v>0.25</v>
@@ -2463,56 +2535,62 @@
       <c r="AG14" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="AH14">
+      <c r="AH14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI14" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ14" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK14">
         <v>200</v>
       </c>
-      <c r="AI14" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ14" t="s">
-        <v>146</v>
-      </c>
-      <c r="AK14">
+      <c r="AL14" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM14">
         <v>10</v>
       </c>
-      <c r="AL14" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM14">
+      <c r="AN14">
         <v>200</v>
       </c>
-      <c r="AN14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AO14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C15" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" t="s">
         <v>110</v>
       </c>
-      <c r="E15" t="s">
-        <v>110</v>
-      </c>
-      <c r="F15" t="s">
-        <v>110</v>
-      </c>
-      <c r="G15" t="s">
-        <v>110</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>111</v>
-      </c>
-      <c r="I15" t="s">
-        <v>112</v>
       </c>
       <c r="J15" s="12">
         <v>0</v>
@@ -2551,7 +2629,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V15" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="W15" s="12">
         <v>7.4999999999999997E-2</v>
@@ -2560,19 +2638,19 @@
         <v>0</v>
       </c>
       <c r="Y15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Z15" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA15" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="AA15" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="AB15">
         <v>20</v>
       </c>
       <c r="AC15" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AD15" s="14">
         <v>0.25</v>
@@ -2586,50 +2664,51 @@
       <c r="AG15" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="AH15">
+      <c r="AH15" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI15" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ15" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK15">
         <v>200</v>
       </c>
-      <c r="AI15" s="2" t="s">
+      <c r="AL15" t="s">
         <v>117</v>
       </c>
-      <c r="AJ15" t="s">
-        <v>118</v>
-      </c>
-      <c r="AK15">
+      <c r="AM15">
         <v>5</v>
       </c>
-      <c r="AL15" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM15">
+      <c r="AN15">
         <v>200</v>
       </c>
-      <c r="AN15">
+      <c r="AO15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP15">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="11">
+    <mergeCell ref="AI4:AK4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="AC4:AF4"/>
+    <mergeCell ref="V4:X4"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
-    <mergeCell ref="AH4:AI4"/>
-    <mergeCell ref="AJ4:AN4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="AC4:AF4"/>
-    <mergeCell ref="V4:X4"/>
   </mergeCells>
-  <dataValidations count="18">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI11 AI14:AI15">
+  <dataValidations count="20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO11 AO14:AO15">
       <formula1>"MA,EAA"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL6:AL11 AL14:AL15">
-      <formula1>"MA,AL"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA14:AA15 AA6:AA11">
@@ -2680,19 +2759,29 @@
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AK6:AK11 AK14:AK15">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AM6:AM11 AM14:AM15">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM6:AM11 AM14:AM15">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN14:AN15 AN6:AN11">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN11 AN14:AN15">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP11 AP14:AP15">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V11 V14:V15"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AH15">
+      <formula1>"TRUE, FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI15">
+      <formula1>"MA,AL,AL_pct"</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ15">
+      <formula1>0</formula1>
+      <formula2>1.5</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2707,25 +2796,25 @@
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
         <v>93</v>
       </c>
-      <c r="C3" t="s">
-        <v>94</v>
-      </c>
       <c r="D3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B4" s="12">
         <v>7.4999999999999997E-2</v>
@@ -2737,9 +2826,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" s="12">
         <v>5.5E-2</v>
@@ -2751,9 +2840,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" s="12">
         <v>7.4999999999999997E-2</v>
@@ -2788,25 +2877,25 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" t="s">
         <v>159</v>
       </c>
-      <c r="C2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" s="18">
         <v>11</v>
@@ -2827,44 +2916,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.5546875"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>105</v>
       </c>
@@ -2901,248 +2990,248 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625"/>
+    <col min="1" max="1" width="23.42578125"/>
     <col min="2" max="2" width="5"/>
-    <col min="3" max="3" width="85.44140625"/>
-    <col min="4" max="1025" width="8.5546875"/>
+    <col min="3" max="3" width="85.42578125"/>
+    <col min="4" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="C4" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="15" t="s">
+    </row>
+    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="C9" t="s">
         <v>135</v>
       </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="C13" t="s">
         <v>138</v>
       </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="C14" t="s">
         <v>140</v>
       </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>110</v>
       </c>
-      <c r="C17" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>143</v>
-      </c>
-      <c r="C18" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>110</v>
-      </c>
-      <c r="C21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>143</v>
-      </c>
-      <c r="C22" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C25" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>143</v>
-      </c>
-      <c r="C26" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>110</v>
-      </c>
-      <c r="C29" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>143</v>
-      </c>
-      <c r="C30" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>118</v>
-      </c>
-      <c r="C33" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>146</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="C37" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="16" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>148</v>
+      </c>
+      <c r="C38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>150</v>
+      </c>
+      <c r="C39" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>152</v>
+      </c>
+      <c r="C40" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>111</v>
       </c>
-      <c r="C37" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>149</v>
-      </c>
-      <c r="C38" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>151</v>
-      </c>
-      <c r="C39" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>153</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="C43" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>112</v>
-      </c>
-      <c r="C43" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the RunControl file
</commit_message>
<xml_diff>
--- a/RunControl_initRuns.xlsx
+++ b/RunControl_initRuns.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Model_Main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\PenSim-Projects\Model_Main\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="205">
   <si>
     <t>Sheet #</t>
   </si>
@@ -556,9 +556,6 @@
     <t>Fixed discount rate 7.5%, fixed investment return  9.5%; smoothed</t>
   </si>
   <si>
-    <t>Fixed discount rate 7.5%, stochastic investment return arithmetic mean 7.5%, sd 12%</t>
-  </si>
-  <si>
     <t>Fixed Return Fixed discount rate and investment return, 7.5% each, with 5-year period of low returns; Smoothed</t>
   </si>
   <si>
@@ -584,6 +581,69 @@
   </si>
   <si>
     <t>MA_0_pct</t>
+  </si>
+  <si>
+    <t>R2F2</t>
+  </si>
+  <si>
+    <t>R2F3</t>
+  </si>
+  <si>
+    <t>R3F3</t>
+  </si>
+  <si>
+    <t>R4F3</t>
+  </si>
+  <si>
+    <t>R5F3</t>
+  </si>
+  <si>
+    <t>R6F3</t>
+  </si>
+  <si>
+    <t>Fixed discount rate 7.5%, stochastic investment return arithmetic mean 7.5%, sd 12%; Smoothed</t>
+  </si>
+  <si>
+    <t>Fixed discount rate 7.5%, fixed investment return 5.5%; Unsmoothed</t>
+  </si>
+  <si>
+    <t>Fixed discount rate 7.5%, fixed investment return  9.5%; Unsmoothed</t>
+  </si>
+  <si>
+    <t>Fixed discount rate 7.5%, stochastic investment return arithmetic mean 7.5%, sd 12%; Unsmoothed</t>
+  </si>
+  <si>
+    <t>Fixed Return Fixed discount rate and investment return, 7.5% each, with 5-year period of low returns; Unsmoothed</t>
+  </si>
+  <si>
+    <t>Fixed Return Fixed discount rate and investment return, 7.5% each, with 5-year period of low contributions; Unsmoothed</t>
+  </si>
+  <si>
+    <t>Fixed discount rate 7.5%, fixed investment return 5.5%; Typical</t>
+  </si>
+  <si>
+    <t>Fixed discount rate 7.5%, fixed investment return  9.5%; Typical</t>
+  </si>
+  <si>
+    <t>Fixed discount rate 7.5%, stochastic investment return arithmetic mean 7.5%, sd 12%; Typical</t>
+  </si>
+  <si>
+    <t>Fixed Return Fixed discount rate and investment return, 7.5% each, with 5-year period of low returns; Typical</t>
+  </si>
+  <si>
+    <t>Fixed Return Fixed discount rate and investment return, 7.5% each, with 5-year period of low contributions; Typical</t>
+  </si>
+  <si>
+    <t>R5F2</t>
+  </si>
+  <si>
+    <t>R6F2</t>
+  </si>
+  <si>
+    <t>R3F2</t>
+  </si>
+  <si>
+    <t>R4F2</t>
   </si>
 </sst>
 </file>
@@ -717,7 +777,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -760,13 +820,11 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -775,14 +833,17 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1144,14 +1205,14 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5703125"/>
-    <col min="2" max="2" width="16.7109375"/>
-    <col min="3" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="7.5546875"/>
+    <col min="2" max="2" width="16.6640625"/>
+    <col min="3" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1159,7 +1220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1167,7 +1228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1175,7 +1236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1202,77 +1263,77 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125"/>
+    <col min="1" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1285,37 +1346,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP15"/>
+  <dimension ref="A1:AP27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="AE6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="S14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AL21" sqref="AL21"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="54.42578125"/>
-    <col min="2" max="2" width="98.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="24.42578125"/>
-    <col min="10" max="11" width="17.42578125"/>
-    <col min="12" max="12" width="16.140625"/>
-    <col min="13" max="14" width="21.42578125"/>
-    <col min="15" max="15" width="24.5703125"/>
+    <col min="1" max="1" width="54.44140625"/>
+    <col min="2" max="2" width="98.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="24.44140625"/>
+    <col min="10" max="11" width="17.44140625"/>
+    <col min="12" max="12" width="16.109375"/>
+    <col min="13" max="14" width="21.44140625"/>
+    <col min="15" max="15" width="24.5546875"/>
     <col min="16" max="16" width="16"/>
-    <col min="17" max="21" width="12.7109375"/>
-    <col min="22" max="22" width="11.140625" customWidth="1"/>
-    <col min="23" max="32" width="12.7109375"/>
+    <col min="17" max="21" width="12.6640625"/>
+    <col min="22" max="22" width="11.109375" customWidth="1"/>
+    <col min="23" max="32" width="12.6640625"/>
     <col min="36" max="36" width="12" customWidth="1"/>
-    <col min="37" max="37" width="12.7109375"/>
-    <col min="38" max="39" width="27.140625"/>
-    <col min="40" max="40" width="26.85546875"/>
+    <col min="37" max="37" width="12.6640625"/>
+    <col min="38" max="39" width="27.109375"/>
+    <col min="40" max="40" width="26.88671875"/>
     <col min="42" max="42" width="16"/>
-    <col min="43" max="1029" width="8.5703125"/>
+    <col min="43" max="1029" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
       <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1325,7 +1386,7 @@
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
     </row>
-    <row r="2" spans="1:42" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -1387,10 +1448,10 @@
         <v>40</v>
       </c>
       <c r="AH2" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AI2" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AJ2" s="6"/>
       <c r="AK2" s="4" t="s">
@@ -1403,7 +1464,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:42" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -1438,7 +1499,7 @@
         <v>53</v>
       </c>
       <c r="AI3" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AJ3" s="4"/>
       <c r="AM3" s="4" t="s">
@@ -1454,20 +1515,20 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:42" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:42" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25" t="s">
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26" t="s">
+      <c r="E4" s="31"/>
+      <c r="F4" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="26"/>
+      <c r="G4" s="32"/>
       <c r="H4" s="27" t="s">
         <v>61</v>
       </c>
@@ -1490,19 +1551,19 @@
       </c>
       <c r="T4" s="28"/>
       <c r="U4" s="28"/>
-      <c r="V4" s="29" t="s">
+      <c r="V4" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="W4" s="29"/>
-      <c r="X4" s="29"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
       <c r="Y4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="24" t="s">
+      <c r="Z4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="AA4" s="24"/>
-      <c r="AB4" s="24"/>
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="29"/>
       <c r="AC4" s="30" t="s">
         <v>68</v>
       </c>
@@ -1511,20 +1572,20 @@
       <c r="AF4" s="30"/>
       <c r="AG4" s="17"/>
       <c r="AH4" s="23"/>
-      <c r="AI4" s="29" t="s">
+      <c r="AI4" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="AJ4" s="29"/>
-      <c r="AK4" s="29"/>
-      <c r="AL4" s="31" t="s">
+      <c r="AJ4" s="26"/>
+      <c r="AK4" s="26"/>
+      <c r="AL4" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="AM4" s="31"/>
-      <c r="AN4" s="31"/>
-      <c r="AO4" s="31"/>
-      <c r="AP4" s="31"/>
-    </row>
-    <row r="5" spans="1:42" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="AM4" s="24"/>
+      <c r="AN4" s="24"/>
+      <c r="AO4" s="24"/>
+      <c r="AP4" s="24"/>
+    </row>
+    <row r="5" spans="1:42" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>71</v>
       </c>
@@ -1625,13 +1686,13 @@
         <v>161</v>
       </c>
       <c r="AH5" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AI5" s="9" t="s">
         <v>106</v>
       </c>
       <c r="AJ5" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AK5" s="9" t="s">
         <v>102</v>
@@ -1652,7 +1713,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>162</v>
       </c>
@@ -1781,7 +1842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>163</v>
       </c>
@@ -1910,7 +1971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>166</v>
       </c>
@@ -2039,12 +2100,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>168</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="C9" s="11" t="b">
         <f>TRUE()</f>
@@ -2168,12 +2229,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>167</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C10" s="11" t="b">
         <f>TRUE()</f>
@@ -2233,7 +2294,7 @@
       <c r="U10" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V10" s="12" t="s">
+      <c r="V10" s="25" t="s">
         <v>157</v>
       </c>
       <c r="W10" s="12">
@@ -2297,12 +2358,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>169</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C11" s="11" t="b">
         <f>TRUE()</f>
@@ -2426,21 +2487,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
       <c r="B12" s="22"/>
       <c r="AH12" s="21"/>
       <c r="AJ12" s="19"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
       <c r="AH13" s="21"/>
       <c r="AJ13" s="19"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>164</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C14" s="11" t="b">
         <f>TRUE()</f>
@@ -2564,12 +2625,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="C15" s="11" t="b">
         <f>TRUE()</f>
@@ -2629,11 +2690,11 @@
       <c r="U15" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V15" s="12" t="s">
+      <c r="V15" t="s">
         <v>160</v>
       </c>
       <c r="W15" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="X15" s="12">
         <v>0</v>
@@ -2642,13 +2703,13 @@
         <v>112</v>
       </c>
       <c r="Z15" s="2" t="s">
-        <v>170</v>
+        <v>113</v>
       </c>
       <c r="AA15" s="2" t="s">
-        <v>171</v>
+        <v>114</v>
       </c>
       <c r="AB15">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AC15" s="2" t="s">
         <v>115</v>
@@ -2678,10 +2739,10 @@
         <v>200</v>
       </c>
       <c r="AL15" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="AM15">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AN15">
         <v>200</v>
@@ -2693,97 +2754,1392 @@
         <v>1</v>
       </c>
     </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>203</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="C16" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" t="s">
+        <v>109</v>
+      </c>
+      <c r="G16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" t="s">
+        <v>110</v>
+      </c>
+      <c r="I16" t="s">
+        <v>111</v>
+      </c>
+      <c r="J16" s="12">
+        <v>0</v>
+      </c>
+      <c r="K16" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L16" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+      <c r="N16">
+        <v>65</v>
+      </c>
+      <c r="O16">
+        <v>65</v>
+      </c>
+      <c r="P16" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q16">
+        <v>10</v>
+      </c>
+      <c r="R16">
+        <v>10</v>
+      </c>
+      <c r="S16" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T16" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U16" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V16" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="W16" s="12">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="X16" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z16" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB16">
+        <v>10</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD16" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE16" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF16" s="14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI16" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ16" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK16">
+        <v>200</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM16">
+        <v>10</v>
+      </c>
+      <c r="AN16">
+        <v>200</v>
+      </c>
+      <c r="AO16" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>204</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="C17" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" t="s">
+        <v>110</v>
+      </c>
+      <c r="I17" t="s">
+        <v>111</v>
+      </c>
+      <c r="J17" s="12">
+        <v>0</v>
+      </c>
+      <c r="K17" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L17" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M17">
+        <v>3</v>
+      </c>
+      <c r="N17">
+        <v>65</v>
+      </c>
+      <c r="O17">
+        <v>65</v>
+      </c>
+      <c r="P17" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q17">
+        <v>10</v>
+      </c>
+      <c r="R17">
+        <v>10</v>
+      </c>
+      <c r="S17" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T17" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U17" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V17" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="W17" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X17" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z17" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB17">
+        <v>10</v>
+      </c>
+      <c r="AC17" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD17" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE17" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF17" s="14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG17" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI17" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ17" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK17">
+        <v>200</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM17">
+        <v>10</v>
+      </c>
+      <c r="AN17">
+        <v>200</v>
+      </c>
+      <c r="AO17" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="C18" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" t="s">
+        <v>110</v>
+      </c>
+      <c r="I18" t="s">
+        <v>111</v>
+      </c>
+      <c r="J18" s="12">
+        <v>0</v>
+      </c>
+      <c r="K18" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L18" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+      <c r="N18">
+        <v>65</v>
+      </c>
+      <c r="O18">
+        <v>65</v>
+      </c>
+      <c r="P18" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q18">
+        <v>10</v>
+      </c>
+      <c r="R18">
+        <v>10</v>
+      </c>
+      <c r="S18" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T18" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U18" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V18" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="W18" s="12">
+        <v>0</v>
+      </c>
+      <c r="X18" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB18">
+        <v>10</v>
+      </c>
+      <c r="AC18" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD18" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE18" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF18" s="14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG18" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI18" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ18" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK18">
+        <v>200</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM18">
+        <v>10</v>
+      </c>
+      <c r="AN18">
+        <v>200</v>
+      </c>
+      <c r="AO18" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>202</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="C19" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19" t="s">
+        <v>110</v>
+      </c>
+      <c r="I19" t="s">
+        <v>111</v>
+      </c>
+      <c r="J19" s="12">
+        <v>0</v>
+      </c>
+      <c r="K19" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M19">
+        <v>3</v>
+      </c>
+      <c r="N19">
+        <v>65</v>
+      </c>
+      <c r="O19">
+        <v>65</v>
+      </c>
+      <c r="P19" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q19">
+        <v>10</v>
+      </c>
+      <c r="R19">
+        <v>10</v>
+      </c>
+      <c r="S19" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T19" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U19" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V19" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="W19" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X19" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA19" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB19">
+        <v>10</v>
+      </c>
+      <c r="AC19" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD19" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE19" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF19" s="14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG19" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH19" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI19" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ19" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK19">
+        <v>200</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM19">
+        <v>10</v>
+      </c>
+      <c r="AN19">
+        <v>200</v>
+      </c>
+      <c r="AO19" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>165</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" t="s">
+        <v>110</v>
+      </c>
+      <c r="I22" t="s">
+        <v>111</v>
+      </c>
+      <c r="J22" s="12">
+        <v>0</v>
+      </c>
+      <c r="K22" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L22" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M22">
+        <v>3</v>
+      </c>
+      <c r="N22">
+        <v>65</v>
+      </c>
+      <c r="O22">
+        <v>65</v>
+      </c>
+      <c r="P22" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q22">
+        <v>10</v>
+      </c>
+      <c r="R22">
+        <v>10</v>
+      </c>
+      <c r="S22" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T22" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U22" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V22" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="W22" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X22" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z22" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA22" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB22">
+        <v>20</v>
+      </c>
+      <c r="AC22" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD22" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE22" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF22" s="14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG22" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI22" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ22" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK22">
+        <v>200</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM22">
+        <v>5</v>
+      </c>
+      <c r="AN22">
+        <v>200</v>
+      </c>
+      <c r="AO22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>185</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="C23" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" t="s">
+        <v>110</v>
+      </c>
+      <c r="I23" t="s">
+        <v>111</v>
+      </c>
+      <c r="J23" s="12">
+        <v>0</v>
+      </c>
+      <c r="K23" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L23" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M23">
+        <v>3</v>
+      </c>
+      <c r="N23">
+        <v>65</v>
+      </c>
+      <c r="O23">
+        <v>65</v>
+      </c>
+      <c r="P23" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q23">
+        <v>10</v>
+      </c>
+      <c r="R23">
+        <v>10</v>
+      </c>
+      <c r="S23" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T23" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U23" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V23" t="s">
+        <v>160</v>
+      </c>
+      <c r="W23" s="12">
+        <v>5.5E-2</v>
+      </c>
+      <c r="X23" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z23" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA23" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB23">
+        <v>20</v>
+      </c>
+      <c r="AC23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD23" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE23" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF23" s="14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG23" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI23" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ23" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK23">
+        <v>200</v>
+      </c>
+      <c r="AL23" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM23">
+        <v>5</v>
+      </c>
+      <c r="AN23">
+        <v>200</v>
+      </c>
+      <c r="AO23" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>186</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="C24" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" t="s">
+        <v>110</v>
+      </c>
+      <c r="I24" t="s">
+        <v>111</v>
+      </c>
+      <c r="J24" s="12">
+        <v>0</v>
+      </c>
+      <c r="K24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L24" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M24">
+        <v>3</v>
+      </c>
+      <c r="N24">
+        <v>65</v>
+      </c>
+      <c r="O24">
+        <v>65</v>
+      </c>
+      <c r="P24" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q24">
+        <v>10</v>
+      </c>
+      <c r="R24">
+        <v>10</v>
+      </c>
+      <c r="S24" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T24" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U24" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V24" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="W24" s="12">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="X24" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z24" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA24" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB24">
+        <v>20</v>
+      </c>
+      <c r="AC24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD24" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE24" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF24" s="14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG24" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI24" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ24" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK24">
+        <v>200</v>
+      </c>
+      <c r="AL24" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM24">
+        <v>5</v>
+      </c>
+      <c r="AN24">
+        <v>200</v>
+      </c>
+      <c r="AO24" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>187</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="C25" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25" t="s">
+        <v>109</v>
+      </c>
+      <c r="H25" t="s">
+        <v>110</v>
+      </c>
+      <c r="I25" t="s">
+        <v>111</v>
+      </c>
+      <c r="J25" s="12">
+        <v>0</v>
+      </c>
+      <c r="K25" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L25" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M25">
+        <v>3</v>
+      </c>
+      <c r="N25">
+        <v>65</v>
+      </c>
+      <c r="O25">
+        <v>65</v>
+      </c>
+      <c r="P25" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q25">
+        <v>10</v>
+      </c>
+      <c r="R25">
+        <v>10</v>
+      </c>
+      <c r="S25" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T25" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U25" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V25" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="W25" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X25" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z25" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA25" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB25">
+        <v>20</v>
+      </c>
+      <c r="AC25" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD25" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE25" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF25" s="14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG25" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI25" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ25" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK25">
+        <v>200</v>
+      </c>
+      <c r="AL25" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM25">
+        <v>5</v>
+      </c>
+      <c r="AN25">
+        <v>200</v>
+      </c>
+      <c r="AO25" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>188</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="C26" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" t="s">
+        <v>109</v>
+      </c>
+      <c r="G26" t="s">
+        <v>109</v>
+      </c>
+      <c r="H26" t="s">
+        <v>110</v>
+      </c>
+      <c r="I26" t="s">
+        <v>111</v>
+      </c>
+      <c r="J26" s="12">
+        <v>0</v>
+      </c>
+      <c r="K26" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L26" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M26">
+        <v>3</v>
+      </c>
+      <c r="N26">
+        <v>65</v>
+      </c>
+      <c r="O26">
+        <v>65</v>
+      </c>
+      <c r="P26" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
+      <c r="R26">
+        <v>10</v>
+      </c>
+      <c r="S26" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T26" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U26" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V26" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="W26" s="12">
+        <v>0</v>
+      </c>
+      <c r="X26" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z26" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA26" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB26">
+        <v>20</v>
+      </c>
+      <c r="AC26" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD26" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE26" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF26" s="14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG26" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI26" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ26" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK26">
+        <v>200</v>
+      </c>
+      <c r="AL26" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM26">
+        <v>5</v>
+      </c>
+      <c r="AN26">
+        <v>200</v>
+      </c>
+      <c r="AO26" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>189</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="C27" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" t="s">
+        <v>109</v>
+      </c>
+      <c r="G27" t="s">
+        <v>109</v>
+      </c>
+      <c r="H27" t="s">
+        <v>110</v>
+      </c>
+      <c r="I27" t="s">
+        <v>111</v>
+      </c>
+      <c r="J27" s="12">
+        <v>0</v>
+      </c>
+      <c r="K27" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L27" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M27">
+        <v>3</v>
+      </c>
+      <c r="N27">
+        <v>65</v>
+      </c>
+      <c r="O27">
+        <v>65</v>
+      </c>
+      <c r="P27" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q27">
+        <v>10</v>
+      </c>
+      <c r="R27">
+        <v>10</v>
+      </c>
+      <c r="S27" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T27" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U27" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V27" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="W27" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X27" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z27" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA27" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB27">
+        <v>20</v>
+      </c>
+      <c r="AC27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD27" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE27" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF27" s="14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG27" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH27" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI27" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ27" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AK27">
+        <v>200</v>
+      </c>
+      <c r="AL27" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM27">
+        <v>5</v>
+      </c>
+      <c r="AN27">
+        <v>200</v>
+      </c>
+      <c r="AO27" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP27">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="AI4:AK4"/>
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AC4:AF4"/>
     <mergeCell ref="V4:X4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <dataValidations count="20">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO11 AO14:AO15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO11 AO22:AO27 AO14:AO19">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA14:AA15 AA6:AA11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6:AA11 AA22:AA27 AA14:AA19">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z14:Z15 Z6:Z11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6:Z11 Z22:Z27 Z14:Z19">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC6:AC11 AC14:AC15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC6:AC11 AC22:AC27 AC14:AC19">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C11 K6:K11 C14:C15 K14:K15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C11 K6:K11 K22:K27 K14:K19 C22:C27 C14:C19">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6:N11 N14:N15">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6:N11 N22:N27 N14:N19">
       <formula1>55</formula1>
       <formula2>65</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="P6:P11 T6:T11 P14:P15 T14:T15">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="P6:P11 T6:T11 T22:T27 T14:T19 P22:P27 P14:P19">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q6:R11 Q14:R15">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q6:R11 Q22:R27 Q14:R19">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="S6:S11 U6:U11 W6:W11 S14:S15 U14:U15 W14:W15">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="S6:S11 U6:U11 W6:W11 W14:W19 S14:S19 U22:U27 U14:U19 S22:S27 W22:W27">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB14:AB15 AB6:AB11">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB6:AB11 AB22:AB27 AB14:AB19">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AD6:AE11 AD14:AE15">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AD6:AE11 AD14:AE19 AD22:AE27">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AF6:AF11 AF14:AF15">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AF6:AF11 AF14:AF19 AF22:AF27">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X6:X11 X14:X15">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X6:X11 X14:X19 X22:X27">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AM6:AM11 AM14:AM15">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AM6:AM11 AM22:AM27 AM14:AM19">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN14:AN15 AN6:AN11">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN11 AN22:AN27 AN14:AN19">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP11 AP14:AP15">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP11 AP22:AP27 AP14:AP19">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V11 V14:V15"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AH15">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V11 V14:V19 V22:V27"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AH19 AG22:AH27">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI19 AI22:AI27">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ15">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ19 AJ22:AJ27">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="V10" location="Returns!A1" display="internal"/>
+    <hyperlink ref="V18" location="Returns!A1" display="internal"/>
+    <hyperlink ref="V26" location="Returns!A1" display="internal"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -2791,15 +4147,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D6"/>
+  <dimension ref="A3:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -2813,7 +4167,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>167</v>
       </c>
@@ -2827,7 +4181,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>167</v>
       </c>
@@ -2841,7 +4195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>167</v>
       </c>
@@ -2855,13 +4209,97 @@
         <v>90</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" s="12">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="12">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B12" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="C4:C6">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="C4:C12">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="B4:B6">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="B4:B12">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
@@ -2872,15 +4310,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D3"/>
+  <dimension ref="A2:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -2894,7 +4332,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>169</v>
       </c>
@@ -2905,6 +4343,34 @@
         <v>5</v>
       </c>
       <c r="D3" s="19">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="18">
+        <v>11</v>
+      </c>
+      <c r="C4" s="18">
+        <v>5</v>
+      </c>
+      <c r="D4" s="19">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5" s="18">
+        <v>11</v>
+      </c>
+      <c r="C5" s="18">
+        <v>5</v>
+      </c>
+      <c r="D5" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -2918,20 +4384,20 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125"/>
+    <col min="1" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>121</v>
       </c>
@@ -2954,7 +4420,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>105</v>
       </c>
@@ -2962,7 +4428,7 @@
         <v>1000</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -2991,30 +4457,30 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125"/>
+    <col min="1" max="1" width="23.44140625"/>
     <col min="2" max="2" width="5"/>
-    <col min="3" max="3" width="85.42578125"/>
-    <col min="4" max="1025" width="8.5703125"/>
+    <col min="3" max="3" width="85.44140625"/>
+    <col min="4" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>128</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>130</v>
       </c>
@@ -3022,12 +4488,12 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -3035,7 +4501,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -3043,7 +4509,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>134</v>
       </c>
@@ -3051,12 +4517,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>115</v>
       </c>
@@ -3064,7 +4530,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -3072,7 +4538,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -3080,12 +4546,12 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>109</v>
       </c>
@@ -3093,7 +4559,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -3101,12 +4567,12 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>109</v>
       </c>
@@ -3114,7 +4580,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>142</v>
       </c>
@@ -3122,12 +4588,12 @@
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>109</v>
       </c>
@@ -3135,7 +4601,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>142</v>
       </c>
@@ -3143,12 +4609,12 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>109</v>
       </c>
@@ -3156,7 +4622,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -3164,12 +4630,12 @@
         <v>143</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>117</v>
       </c>
@@ -3177,7 +4643,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>145</v>
       </c>
@@ -3185,12 +4651,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -3198,7 +4664,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>148</v>
       </c>
@@ -3206,7 +4672,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>150</v>
       </c>
@@ -3214,7 +4680,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -3222,12 +4688,12 @@
         <v>153</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
Take the calculation of some variables out of the loop
</commit_message>
<xml_diff>
--- a/RunControl_initRuns.xlsx
+++ b/RunControl_initRuns.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -1348,11 +1348,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="S14" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2529,7 +2529,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14" s="12">
         <v>1.4999999999999999E-2</v>
@@ -2658,7 +2658,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="12">
         <v>1.4999999999999999E-2</v>
@@ -2787,7 +2787,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="12">
         <v>1.4999999999999999E-2</v>
@@ -2916,7 +2916,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="12">
         <v>1.4999999999999999E-2</v>
@@ -3045,7 +3045,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18" s="12">
         <v>1.4999999999999999E-2</v>
@@ -3174,7 +3174,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="12">
         <v>1.4999999999999999E-2</v>
@@ -3303,7 +3303,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22" s="12">
         <v>1.4999999999999999E-2</v>
@@ -3432,7 +3432,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23" s="12">
         <v>1.4999999999999999E-2</v>
@@ -3561,7 +3561,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24" s="12">
         <v>1.4999999999999999E-2</v>
@@ -3690,7 +3690,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" s="12">
         <v>1.4999999999999999E-2</v>
@@ -3819,7 +3819,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26" s="12">
         <v>1.4999999999999999E-2</v>
@@ -3948,7 +3948,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27" s="12">
         <v>1.4999999999999999E-2</v>
@@ -4075,7 +4075,7 @@
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C11 K6:K11 K22:K27 K14:K19 C22:C27 C14:C19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C11 K6:K11 K14:K19 C14:C19 C22:C27 K22:K27">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4383,8 +4383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4422,10 +4422,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="B3">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="C3">
         <v>6</v>

</xml_diff>

<commit_message>
can control if EEC can be reduced when ADC is low
</commit_message>
<xml_diff>
--- a/RunControl_initRuns.xlsx
+++ b/RunControl_initRuns.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="207">
   <si>
     <t>Sheet #</t>
   </si>
@@ -644,6 +644,12 @@
   </si>
   <si>
     <t>R4F2</t>
+  </si>
+  <si>
+    <t>EEC_fixed</t>
+  </si>
+  <si>
+    <t>whether EEC is fixed as a % of payroll</t>
   </si>
 </sst>
 </file>
@@ -777,7 +783,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -824,7 +830,17 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -833,16 +849,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1346,13 +1356,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP27"/>
+  <dimension ref="A1:AQ27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="AD18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
+      <selection pane="bottomRight" activeCell="AJ21" sqref="AJ21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1368,15 +1378,16 @@
     <col min="17" max="21" width="12.6640625"/>
     <col min="22" max="22" width="11.109375" customWidth="1"/>
     <col min="23" max="32" width="12.6640625"/>
-    <col min="36" max="36" width="12" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625"/>
-    <col min="38" max="39" width="27.109375"/>
-    <col min="40" max="40" width="26.88671875"/>
-    <col min="42" max="42" width="16"/>
-    <col min="43" max="1029" width="8.5546875"/>
+    <col min="35" max="35" width="9" customWidth="1"/>
+    <col min="37" max="37" width="12" customWidth="1"/>
+    <col min="38" max="38" width="12.6640625"/>
+    <col min="39" max="40" width="27.109375"/>
+    <col min="41" max="41" width="26.88671875"/>
+    <col min="43" max="43" width="16"/>
+    <col min="44" max="1030" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
       <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1385,8 +1396,9 @@
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
-    </row>
-    <row r="2" spans="1:42" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AI1" s="1"/>
+    </row>
+    <row r="2" spans="1:43" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -1450,21 +1462,24 @@
       <c r="AH2" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AI2" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="AJ2" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="AJ2" s="6"/>
-      <c r="AK2" s="4" t="s">
+      <c r="AK2" s="6"/>
+      <c r="AL2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AL2" s="6"/>
       <c r="AM2" s="6"/>
-      <c r="AO2" s="6"/>
-      <c r="AP2" s="4" t="s">
+      <c r="AN2" s="6"/>
+      <c r="AP2" s="6"/>
+      <c r="AQ2" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:42" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -1498,94 +1513,95 @@
       <c r="AE3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AI3" s="4" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="AJ3" s="4"/>
-      <c r="AM3" s="4" t="s">
+      <c r="AK3" s="4"/>
+      <c r="AN3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AN3" s="4" t="s">
+      <c r="AO3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AO3" s="4" t="s">
+      <c r="AP3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AP3" s="4" t="s">
+      <c r="AQ3" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:42" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
+    <row r="4" spans="1:43" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="31" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="32" t="s">
+      <c r="E4" s="29"/>
+      <c r="F4" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="32"/>
-      <c r="H4" s="27" t="s">
+      <c r="G4" s="30"/>
+      <c r="H4" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="28" t="s">
+      <c r="I4" s="31"/>
+      <c r="J4" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="27" t="s">
+      <c r="K4" s="32"/>
+      <c r="L4" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="28" t="s">
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="28"/>
-      <c r="U4" s="28"/>
-      <c r="V4" s="26" t="s">
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="33"/>
       <c r="Y4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="29" t="s">
+      <c r="Z4" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="AA4" s="29"/>
-      <c r="AB4" s="29"/>
-      <c r="AC4" s="30" t="s">
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="AD4" s="30"/>
-      <c r="AE4" s="30"/>
-      <c r="AF4" s="30"/>
+      <c r="AD4" s="34"/>
+      <c r="AE4" s="34"/>
+      <c r="AF4" s="34"/>
       <c r="AG4" s="17"/>
-      <c r="AH4" s="23"/>
-      <c r="AI4" s="26" t="s">
+      <c r="AH4" s="27"/>
+      <c r="AI4" s="23"/>
+      <c r="AJ4" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="AJ4" s="26"/>
-      <c r="AK4" s="26"/>
-      <c r="AL4" s="24" t="s">
+      <c r="AK4" s="33"/>
+      <c r="AL4" s="33"/>
+      <c r="AM4" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="AM4" s="24"/>
       <c r="AN4" s="24"/>
       <c r="AO4" s="24"/>
       <c r="AP4" s="24"/>
-    </row>
-    <row r="5" spans="1:42" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AQ4" s="24"/>
+    </row>
+    <row r="5" spans="1:43" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>71</v>
       </c>
@@ -1689,31 +1705,34 @@
         <v>180</v>
       </c>
       <c r="AI5" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AJ5" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="AJ5" s="9" t="s">
+      <c r="AK5" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="AK5" s="9" t="s">
+      <c r="AL5" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AL5" s="9" t="s">
+      <c r="AM5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="AM5" s="9" t="s">
+      <c r="AN5" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="AN5" s="9" t="s">
+      <c r="AO5" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="AO5" s="9" t="s">
+      <c r="AP5" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="AP5" s="9" t="s">
+      <c r="AQ5" s="9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>162</v>
       </c>
@@ -1746,7 +1765,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6" s="12">
         <v>1.4999999999999999E-2</v>
@@ -1809,7 +1828,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF6" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG6" s="20" t="b">
         <v>0</v>
@@ -1817,32 +1836,35 @@
       <c r="AH6" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI6" s="2" t="s">
+      <c r="AI6" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ6" s="19">
+      <c r="AK6" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK6">
+      <c r="AL6">
         <v>200</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AM6" t="s">
         <v>117</v>
       </c>
-      <c r="AM6">
-        <v>10</v>
-      </c>
       <c r="AN6">
+        <v>10</v>
+      </c>
+      <c r="AO6">
         <v>200</v>
       </c>
-      <c r="AO6" s="2" t="s">
+      <c r="AP6" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>163</v>
       </c>
@@ -1874,8 +1896,8 @@
       <c r="J7" s="12">
         <v>0</v>
       </c>
-      <c r="K7" s="13" t="b">
-        <v>1</v>
+      <c r="K7" s="21" t="b">
+        <v>0</v>
       </c>
       <c r="L7" s="12">
         <v>1.4999999999999999E-2</v>
@@ -1938,7 +1960,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF7" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG7" s="21" t="b">
         <v>0</v>
@@ -1946,32 +1968,35 @@
       <c r="AH7" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI7" s="2" t="s">
+      <c r="AI7" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ7" s="19">
+      <c r="AK7" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK7">
+      <c r="AL7">
         <v>200</v>
       </c>
-      <c r="AL7" t="s">
+      <c r="AM7" t="s">
         <v>117</v>
       </c>
-      <c r="AM7">
-        <v>10</v>
-      </c>
       <c r="AN7">
+        <v>10</v>
+      </c>
+      <c r="AO7">
         <v>200</v>
       </c>
-      <c r="AO7" s="2" t="s">
+      <c r="AP7" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>166</v>
       </c>
@@ -2003,8 +2028,8 @@
       <c r="J8" s="12">
         <v>0</v>
       </c>
-      <c r="K8" s="13" t="b">
-        <v>1</v>
+      <c r="K8" s="21" t="b">
+        <v>0</v>
       </c>
       <c r="L8" s="12">
         <v>1.4999999999999999E-2</v>
@@ -2067,7 +2092,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF8" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG8" s="21" t="b">
         <v>0</v>
@@ -2075,32 +2100,35 @@
       <c r="AH8" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI8" s="2" t="s">
+      <c r="AI8" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ8" s="19">
+      <c r="AK8" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK8">
+      <c r="AL8">
         <v>200</v>
       </c>
-      <c r="AL8" t="s">
+      <c r="AM8" t="s">
         <v>117</v>
       </c>
-      <c r="AM8">
-        <v>10</v>
-      </c>
       <c r="AN8">
+        <v>10</v>
+      </c>
+      <c r="AO8">
         <v>200</v>
       </c>
-      <c r="AO8" s="2" t="s">
+      <c r="AP8" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>168</v>
       </c>
@@ -2133,7 +2161,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="12">
         <v>1.4999999999999999E-2</v>
@@ -2196,7 +2224,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF9" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG9" s="21" t="b">
         <v>0</v>
@@ -2204,32 +2232,35 @@
       <c r="AH9" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI9" s="2" t="s">
+      <c r="AI9" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ9" s="19">
+      <c r="AK9" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK9">
+      <c r="AL9">
         <v>200</v>
       </c>
-      <c r="AL9" t="s">
+      <c r="AM9" t="s">
         <v>117</v>
       </c>
-      <c r="AM9">
-        <v>10</v>
-      </c>
       <c r="AN9">
+        <v>10</v>
+      </c>
+      <c r="AO9">
         <v>200</v>
       </c>
-      <c r="AO9" s="2" t="s">
+      <c r="AP9" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>167</v>
       </c>
@@ -2262,7 +2293,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" s="12">
         <v>1.4999999999999999E-2</v>
@@ -2325,7 +2356,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF10" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG10" s="21" t="b">
         <v>0</v>
@@ -2333,32 +2364,35 @@
       <c r="AH10" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI10" s="2" t="s">
+      <c r="AI10" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ10" s="19">
+      <c r="AK10" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK10">
+      <c r="AL10">
         <v>200</v>
       </c>
-      <c r="AL10" t="s">
+      <c r="AM10" t="s">
         <v>117</v>
       </c>
-      <c r="AM10">
-        <v>10</v>
-      </c>
       <c r="AN10">
+        <v>10</v>
+      </c>
+      <c r="AO10">
         <v>200</v>
       </c>
-      <c r="AO10" s="2" t="s">
+      <c r="AP10" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>169</v>
       </c>
@@ -2391,7 +2425,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="12">
         <v>1.4999999999999999E-2</v>
@@ -2454,7 +2488,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF11" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG11" s="21" t="b">
         <v>1</v>
@@ -2462,41 +2496,48 @@
       <c r="AH11" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI11" s="2" t="s">
+      <c r="AI11" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ11" s="19">
+      <c r="AK11" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK11">
+      <c r="AL11">
         <v>200</v>
       </c>
-      <c r="AL11" t="s">
+      <c r="AM11" t="s">
         <v>117</v>
       </c>
-      <c r="AM11">
-        <v>10</v>
-      </c>
       <c r="AN11">
+        <v>10</v>
+      </c>
+      <c r="AO11">
         <v>200</v>
       </c>
-      <c r="AO11" s="2" t="s">
+      <c r="AP11" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B12" s="22"/>
+      <c r="AF12" s="26"/>
       <c r="AH12" s="21"/>
-      <c r="AJ12" s="19"/>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AI12" s="21"/>
+      <c r="AK12" s="19"/>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="AF13" s="26"/>
       <c r="AH13" s="21"/>
-      <c r="AJ13" s="19"/>
-    </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AI13" s="21"/>
+      <c r="AK13" s="19"/>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>164</v>
       </c>
@@ -2592,7 +2633,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF14" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG14" s="21" t="b">
         <v>0</v>
@@ -2600,32 +2641,35 @@
       <c r="AH14" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI14" s="2" t="s">
+      <c r="AI14" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ14" s="19">
+      <c r="AK14" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK14">
+      <c r="AL14">
         <v>200</v>
       </c>
-      <c r="AL14" t="s">
+      <c r="AM14" t="s">
         <v>145</v>
       </c>
-      <c r="AM14">
-        <v>10</v>
-      </c>
       <c r="AN14">
+        <v>10</v>
+      </c>
+      <c r="AO14">
         <v>200</v>
       </c>
-      <c r="AO14" s="2" t="s">
+      <c r="AP14" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>184</v>
       </c>
@@ -2721,7 +2765,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF15" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG15" s="21" t="b">
         <v>0</v>
@@ -2729,32 +2773,35 @@
       <c r="AH15" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI15" s="2" t="s">
+      <c r="AI15" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ15" s="19">
+      <c r="AK15" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK15">
+      <c r="AL15">
         <v>200</v>
       </c>
-      <c r="AL15" t="s">
+      <c r="AM15" t="s">
         <v>145</v>
       </c>
-      <c r="AM15">
-        <v>10</v>
-      </c>
       <c r="AN15">
+        <v>10</v>
+      </c>
+      <c r="AO15">
         <v>200</v>
       </c>
-      <c r="AO15" s="2" t="s">
+      <c r="AP15" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>203</v>
       </c>
@@ -2850,7 +2897,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF16" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG16" s="21" t="b">
         <v>0</v>
@@ -2858,32 +2905,35 @@
       <c r="AH16" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI16" s="2" t="s">
+      <c r="AI16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ16" s="19">
+      <c r="AK16" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK16">
+      <c r="AL16">
         <v>200</v>
       </c>
-      <c r="AL16" t="s">
+      <c r="AM16" t="s">
         <v>145</v>
       </c>
-      <c r="AM16">
-        <v>10</v>
-      </c>
       <c r="AN16">
+        <v>10</v>
+      </c>
+      <c r="AO16">
         <v>200</v>
       </c>
-      <c r="AO16" s="2" t="s">
+      <c r="AP16" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>204</v>
       </c>
@@ -2979,7 +3029,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF17" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG17" s="21" t="b">
         <v>0</v>
@@ -2987,32 +3037,35 @@
       <c r="AH17" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI17" s="2" t="s">
+      <c r="AI17" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ17" s="19">
+      <c r="AK17" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK17">
+      <c r="AL17">
         <v>200</v>
       </c>
-      <c r="AL17" t="s">
+      <c r="AM17" t="s">
         <v>145</v>
       </c>
-      <c r="AM17">
-        <v>10</v>
-      </c>
       <c r="AN17">
+        <v>10</v>
+      </c>
+      <c r="AO17">
         <v>200</v>
       </c>
-      <c r="AO17" s="2" t="s">
+      <c r="AP17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>201</v>
       </c>
@@ -3108,7 +3161,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF18" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG18" s="21" t="b">
         <v>0</v>
@@ -3116,32 +3169,35 @@
       <c r="AH18" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI18" s="2" t="s">
+      <c r="AI18" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ18" s="19">
+      <c r="AK18" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK18">
+      <c r="AL18">
         <v>200</v>
       </c>
-      <c r="AL18" t="s">
+      <c r="AM18" t="s">
         <v>145</v>
       </c>
-      <c r="AM18">
-        <v>10</v>
-      </c>
       <c r="AN18">
+        <v>10</v>
+      </c>
+      <c r="AO18">
         <v>200</v>
       </c>
-      <c r="AO18" s="2" t="s">
+      <c r="AP18" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>202</v>
       </c>
@@ -3237,7 +3293,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF19" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG19" s="21" t="b">
         <v>1</v>
@@ -3245,32 +3301,41 @@
       <c r="AH19" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI19" s="2" t="s">
+      <c r="AI19" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ19" s="19">
+      <c r="AK19" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK19">
+      <c r="AL19">
         <v>200</v>
       </c>
-      <c r="AL19" t="s">
+      <c r="AM19" t="s">
         <v>145</v>
       </c>
-      <c r="AM19">
-        <v>10</v>
-      </c>
       <c r="AN19">
+        <v>10</v>
+      </c>
+      <c r="AO19">
         <v>200</v>
       </c>
-      <c r="AO19" s="2" t="s">
+      <c r="AP19" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="AF20" s="26"/>
+    </row>
+    <row r="21" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="AF21" s="26"/>
+    </row>
+    <row r="22" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>165</v>
       </c>
@@ -3366,7 +3431,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF22" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG22" s="21" t="b">
         <v>0</v>
@@ -3374,32 +3439,35 @@
       <c r="AH22" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI22" s="2" t="s">
+      <c r="AI22" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ22" s="19">
+      <c r="AK22" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK22">
+      <c r="AL22">
         <v>200</v>
       </c>
-      <c r="AL22" t="s">
+      <c r="AM22" t="s">
         <v>117</v>
       </c>
-      <c r="AM22">
+      <c r="AN22">
         <v>5</v>
       </c>
-      <c r="AN22">
+      <c r="AO22">
         <v>200</v>
       </c>
-      <c r="AO22" s="2" t="s">
+      <c r="AP22" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>185</v>
       </c>
@@ -3495,7 +3563,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF23" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG23" s="21" t="b">
         <v>0</v>
@@ -3503,32 +3571,35 @@
       <c r="AH23" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI23" s="2" t="s">
+      <c r="AI23" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ23" s="19">
+      <c r="AK23" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK23">
+      <c r="AL23">
         <v>200</v>
       </c>
-      <c r="AL23" t="s">
+      <c r="AM23" t="s">
         <v>117</v>
       </c>
-      <c r="AM23">
+      <c r="AN23">
         <v>5</v>
       </c>
-      <c r="AN23">
+      <c r="AO23">
         <v>200</v>
       </c>
-      <c r="AO23" s="2" t="s">
+      <c r="AP23" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>186</v>
       </c>
@@ -3624,7 +3695,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF24" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG24" s="21" t="b">
         <v>0</v>
@@ -3632,32 +3703,35 @@
       <c r="AH24" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI24" s="2" t="s">
+      <c r="AI24" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ24" s="19">
+      <c r="AK24" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK24">
+      <c r="AL24">
         <v>200</v>
       </c>
-      <c r="AL24" t="s">
+      <c r="AM24" t="s">
         <v>117</v>
       </c>
-      <c r="AM24">
+      <c r="AN24">
         <v>5</v>
       </c>
-      <c r="AN24">
+      <c r="AO24">
         <v>200</v>
       </c>
-      <c r="AO24" s="2" t="s">
+      <c r="AP24" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>187</v>
       </c>
@@ -3753,7 +3827,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF25" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG25" s="21" t="b">
         <v>0</v>
@@ -3761,32 +3835,35 @@
       <c r="AH25" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI25" s="2" t="s">
+      <c r="AI25" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ25" s="19">
+      <c r="AK25" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK25">
+      <c r="AL25">
         <v>200</v>
       </c>
-      <c r="AL25" t="s">
+      <c r="AM25" t="s">
         <v>117</v>
       </c>
-      <c r="AM25">
+      <c r="AN25">
         <v>5</v>
       </c>
-      <c r="AN25">
+      <c r="AO25">
         <v>200</v>
       </c>
-      <c r="AO25" s="2" t="s">
+      <c r="AP25" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>188</v>
       </c>
@@ -3882,7 +3959,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF26" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG26" s="21" t="b">
         <v>0</v>
@@ -3890,32 +3967,35 @@
       <c r="AH26" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI26" s="2" t="s">
+      <c r="AI26" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ26" s="19">
+      <c r="AK26" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK26">
+      <c r="AL26">
         <v>200</v>
       </c>
-      <c r="AL26" t="s">
+      <c r="AM26" t="s">
         <v>117</v>
       </c>
-      <c r="AM26">
+      <c r="AN26">
         <v>5</v>
       </c>
-      <c r="AN26">
+      <c r="AO26">
         <v>200</v>
       </c>
-      <c r="AO26" s="2" t="s">
+      <c r="AP26" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AQ26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>189</v>
       </c>
@@ -4011,7 +4091,7 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="AF27" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AG27" s="21" t="b">
         <v>1</v>
@@ -4019,47 +4099,50 @@
       <c r="AH27" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="AI27" s="2" t="s">
+      <c r="AI27" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AJ27" s="19">
+      <c r="AK27" s="19">
         <v>0.8</v>
       </c>
-      <c r="AK27">
+      <c r="AL27">
         <v>200</v>
       </c>
-      <c r="AL27" t="s">
+      <c r="AM27" t="s">
         <v>117</v>
       </c>
-      <c r="AM27">
+      <c r="AN27">
         <v>5</v>
       </c>
-      <c r="AN27">
+      <c r="AO27">
         <v>200</v>
       </c>
-      <c r="AO27" s="2" t="s">
+      <c r="AP27" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP27">
+      <c r="AQ27">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AJ4:AL4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="AC4:AF4"/>
+    <mergeCell ref="V4:X4"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
-    <mergeCell ref="AI4:AK4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="AC4:AF4"/>
-    <mergeCell ref="V4:X4"/>
   </mergeCells>
   <dataValidations count="20">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO11 AO22:AO27 AO14:AO19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP11 AP22:AP27 AP14:AP19">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4075,7 +4158,7 @@
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C11 K6:K11 K14:K19 C14:C19 C22:C27 K22:K27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C11 K22:K27 K14:K19 C14:C19 C22:C27 K6:K11">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4111,26 +4194,26 @@
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AM6:AM11 AM22:AM27 AM14:AM19">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AN6:AN11 AN22:AN27 AN14:AN19">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN11 AN22:AN27 AN14:AN19">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO11 AO22:AO27 AO14:AO19">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP11 AP22:AP27 AP14:AP19">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ6:AQ11 AQ22:AQ27 AQ14:AQ19">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V11 V14:V19 V22:V27"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AH19 AG22:AH27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG22:AI27 AG6:AI19">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI19 AI22:AI27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ19 AJ22:AJ27">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ19 AJ22:AJ27">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK19 AK22:AK27">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
@@ -4383,7 +4466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -4425,7 +4508,7 @@
         <v>80</v>
       </c>
       <c r="B3">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="C3">
         <v>6</v>

</xml_diff>

<commit_message>
fix a bug about nsim
</commit_message>
<xml_diff>
--- a/RunControl_initRuns.xlsx
+++ b/RunControl_initRuns.xlsx
@@ -783,7 +783,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -834,7 +834,19 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -843,18 +855,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1359,10 +1360,10 @@
   <dimension ref="A1:AQ27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="AD18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="I6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AJ21" sqref="AJ21"/>
+      <selection pane="bottomRight" activeCell="AK16" sqref="AK16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1398,7 +1399,7 @@
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
     </row>
-    <row r="2" spans="1:43" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:43" s="4" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -1479,7 +1480,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:43" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -1530,69 +1531,69 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:43" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:43" s="8" customFormat="1" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="29" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31" t="s">
+      <c r="G4" s="34"/>
+      <c r="H4" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="32" t="s">
+      <c r="I4" s="29"/>
+      <c r="J4" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="31" t="s">
+      <c r="K4" s="30"/>
+      <c r="L4" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="32" t="s">
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="33" t="s">
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="W4" s="33"/>
-      <c r="X4" s="33"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
       <c r="Y4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="28" t="s">
+      <c r="Z4" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="AA4" s="28"/>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="34" t="s">
+      <c r="AA4" s="31"/>
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
+      <c r="AD4" s="32"/>
+      <c r="AE4" s="32"/>
+      <c r="AF4" s="32"/>
       <c r="AG4" s="17"/>
       <c r="AH4" s="27"/>
       <c r="AI4" s="23"/>
-      <c r="AJ4" s="33" t="s">
+      <c r="AJ4" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="AK4" s="33"/>
-      <c r="AL4" s="33"/>
+      <c r="AK4" s="28"/>
+      <c r="AL4" s="28"/>
       <c r="AM4" s="24" t="s">
         <v>70</v>
       </c>
@@ -1768,7 +1769,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M6">
         <v>3</v>
@@ -1900,7 +1901,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M7">
         <v>3</v>
@@ -2032,7 +2033,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M8">
         <v>3</v>
@@ -2164,7 +2165,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M9">
         <v>3</v>
@@ -2296,7 +2297,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M10">
         <v>3</v>
@@ -2428,7 +2429,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M11">
         <v>3</v>
@@ -2526,12 +2527,14 @@
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B12" s="22"/>
+      <c r="L12" s="35"/>
       <c r="AF12" s="26"/>
       <c r="AH12" s="21"/>
       <c r="AI12" s="21"/>
       <c r="AK12" s="19"/>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="L13" s="35"/>
       <c r="AF13" s="26"/>
       <c r="AH13" s="21"/>
       <c r="AI13" s="21"/>
@@ -2573,7 +2576,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M14">
         <v>3</v>
@@ -2705,7 +2708,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M15">
         <v>3</v>
@@ -2837,7 +2840,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M16">
         <v>3</v>
@@ -2969,7 +2972,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M17">
         <v>3</v>
@@ -3101,7 +3104,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M18">
         <v>3</v>
@@ -3233,7 +3236,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M19">
         <v>3</v>
@@ -3330,9 +3333,11 @@
       </c>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="L20" s="35"/>
       <c r="AF20" s="26"/>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="L21" s="35"/>
       <c r="AF21" s="26"/>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.3">
@@ -3371,7 +3376,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M22">
         <v>3</v>
@@ -3503,7 +3508,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M23">
         <v>3</v>
@@ -3635,7 +3640,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M24">
         <v>3</v>
@@ -3767,7 +3772,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M25">
         <v>3</v>
@@ -3899,7 +3904,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M26">
         <v>3</v>
@@ -4031,7 +4036,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="12">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M27">
         <v>3</v>
@@ -4129,17 +4134,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="AJ4:AL4"/>
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AC4:AF4"/>
     <mergeCell ref="V4:X4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <dataValidations count="20">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP11 AP22:AP27 AP14:AP19">
@@ -4232,7 +4237,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -4289,7 +4296,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -4331,7 +4338,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -4373,7 +4380,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -4467,7 +4474,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4511,7 +4518,7 @@
         <v>1000</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -4536,8 +4543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C48:C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>